<commit_message>
feat: add nasddaq100stocks data
</commit_message>
<xml_diff>
--- a/nasdaq_100_stocks.xlsx
+++ b/nasdaq_100_stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danfr\Desktop\Net Worth\Coding\Python\intermediate\stanproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E374B6-7267-43F2-8EE2-AA95A9F04776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5395AE61-BDB5-4F99-9200-9CD170EF2358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,10 +930,10 @@
   <dimension ref="A1:M1101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>